<commit_message>
Created interface to ask for and create invoice xlsx
</commit_message>
<xml_diff>
--- a/python/comp_230/store_db.xlsx
+++ b/python/comp_230/store_db.xlsx
@@ -1788,14 +1788,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G10:G11"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" customWidth="1"/>
@@ -1851,7 +1852,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -1865,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -1879,10 +1880,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1893,10 +1894,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1904,13 +1905,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,13 +1919,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1935,10 +1936,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,7 +1950,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -1963,10 +1964,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1974,13 +1975,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1988,13 +1989,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2002,10 +2003,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
@@ -2016,10 +2017,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>
@@ -2030,13 +2031,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2047,7 +2048,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1">
         <v>3</v>
@@ -2058,10 +2059,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
@@ -2072,10 +2073,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D20" s="1">
         <v>3</v>
@@ -2086,10 +2087,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1">
         <v>3</v>
@@ -2103,10 +2104,10 @@
         <v>5</v>
       </c>
       <c r="C22" s="1">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2117,10 +2118,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,7 +2132,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1">
         <v>3</v>
@@ -2145,10 +2146,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="1">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2159,10 +2160,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2173,10 +2174,10 @@
         <v>5</v>
       </c>
       <c r="C27" s="1">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D27" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2184,13 +2185,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2198,13 +2199,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,13 +2213,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2226,10 +2227,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C31" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D31" s="1">
         <v>4</v>
@@ -2240,13 +2241,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C32" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D32" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2254,10 +2255,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C33" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D33" s="1">
         <v>3</v>
@@ -2271,10 +2272,10 @@
         <v>7</v>
       </c>
       <c r="C34" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D34" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2285,10 +2286,10 @@
         <v>7</v>
       </c>
       <c r="C35" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2299,10 +2300,10 @@
         <v>7</v>
       </c>
       <c r="C36" s="1">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D36" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2310,13 +2311,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C37" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D37" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2324,10 +2325,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C38" s="1">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -2338,13 +2339,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C39" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2352,13 +2353,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C40" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D40" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2369,10 +2370,10 @@
         <v>9</v>
       </c>
       <c r="C41" s="1">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D41" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2380,10 +2381,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C42" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -2394,10 +2395,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C43" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" s="1">
         <v>3</v>
@@ -2408,10 +2409,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C44" s="1">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D44" s="1">
         <v>4</v>
@@ -2425,10 +2426,10 @@
         <v>10</v>
       </c>
       <c r="C45" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D45" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2439,10 +2440,10 @@
         <v>10</v>
       </c>
       <c r="C46" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D46" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2450,13 +2451,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C47" s="1">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D47" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2464,13 +2465,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C48" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D48" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2478,10 +2479,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C49" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D49" s="1">
         <v>2</v>
@@ -2492,13 +2493,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C50" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D50" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2506,13 +2507,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C51" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D51" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2520,13 +2521,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="1">
+        <v>12</v>
+      </c>
+      <c r="C52" s="1">
         <v>11</v>
       </c>
-      <c r="C52" s="1">
-        <v>17</v>
-      </c>
       <c r="D52" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2537,10 +2538,10 @@
         <v>12</v>
       </c>
       <c r="C53" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2548,13 +2549,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C54" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D54" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2562,13 +2563,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C55" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D55" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2576,13 +2577,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C56" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D56" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2593,10 +2594,10 @@
         <v>13</v>
       </c>
       <c r="C57" s="1">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D57" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2607,10 +2608,10 @@
         <v>13</v>
       </c>
       <c r="C58" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D58" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2621,10 +2622,10 @@
         <v>13</v>
       </c>
       <c r="C59" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D59" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2635,10 +2636,10 @@
         <v>13</v>
       </c>
       <c r="C60" s="1">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D60" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2649,10 +2650,10 @@
         <v>13</v>
       </c>
       <c r="C61" s="1">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D61" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2663,10 +2664,10 @@
         <v>13</v>
       </c>
       <c r="C62" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D62" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2677,7 +2678,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D63" s="1">
         <v>1</v>
@@ -2688,13 +2689,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C64" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D64" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2702,13 +2703,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C65" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D65" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2716,13 +2717,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C66" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D66" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2733,10 +2734,10 @@
         <v>14</v>
       </c>
       <c r="C67" s="1">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D67" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2747,10 +2748,10 @@
         <v>14</v>
       </c>
       <c r="C68" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D68" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2761,10 +2762,10 @@
         <v>14</v>
       </c>
       <c r="C69" s="1">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D69" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2772,13 +2773,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C70" s="1">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D70" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2786,13 +2787,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C71" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D71" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2800,13 +2801,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C72" s="1">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D72" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2817,10 +2818,10 @@
         <v>15</v>
       </c>
       <c r="C73" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D73" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2831,10 +2832,10 @@
         <v>15</v>
       </c>
       <c r="C74" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D74" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2845,10 +2846,10 @@
         <v>15</v>
       </c>
       <c r="C75" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D75" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2859,7 +2860,7 @@
         <v>15</v>
       </c>
       <c r="C76" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
@@ -2870,10 +2871,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C77" s="1">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D77" s="1">
         <v>2</v>
@@ -2884,13 +2885,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C78" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D78" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2898,10 +2899,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C79" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D79" s="1">
         <v>1</v>
@@ -2915,10 +2916,10 @@
         <v>16</v>
       </c>
       <c r="C80" s="1">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D80" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2929,10 +2930,10 @@
         <v>16</v>
       </c>
       <c r="C81" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D81" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2940,13 +2941,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C82" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D82" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2954,10 +2955,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C83" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D83" s="1">
         <v>4</v>
@@ -2968,13 +2969,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C84" s="1">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D84" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2985,10 +2986,10 @@
         <v>17</v>
       </c>
       <c r="C85" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D85" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2996,13 +2997,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C86" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D86" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3010,7 +3011,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C87" s="1">
         <v>19</v>
@@ -3024,13 +3025,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C88" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D88" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -3038,13 +3039,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C89" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D89" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3052,10 +3053,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C90" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D90" s="1">
         <v>1</v>
@@ -3066,13 +3067,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C91" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D91" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -3080,13 +3081,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C92" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D92" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3094,13 +3095,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C93" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D93" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -3111,10 +3112,10 @@
         <v>20</v>
       </c>
       <c r="C94" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D94" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3125,10 +3126,10 @@
         <v>20</v>
       </c>
       <c r="C95" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D95" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3139,7 +3140,7 @@
         <v>20</v>
       </c>
       <c r="C96" s="1">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D96" s="1">
         <v>4</v>
@@ -3153,10 +3154,10 @@
         <v>20</v>
       </c>
       <c r="C97" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D97" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3167,51 +3168,9 @@
         <v>20</v>
       </c>
       <c r="C98" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D98" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>98</v>
-      </c>
-      <c r="B99" s="1">
-        <v>20</v>
-      </c>
-      <c r="C99" s="1">
-        <v>9</v>
-      </c>
-      <c r="D99" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>99</v>
-      </c>
-      <c r="B100" s="1">
-        <v>20</v>
-      </c>
-      <c r="C100" s="1">
-        <v>19</v>
-      </c>
-      <c r="D100" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>100</v>
-      </c>
-      <c r="B101" s="1">
-        <v>20</v>
-      </c>
-      <c r="C101" s="1">
-        <v>14</v>
-      </c>
-      <c r="D101" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>